<commit_message>
Made some changes to the excels
</commit_message>
<xml_diff>
--- a/docs/Manual Test - Server close.xlsx
+++ b/docs/Manual Test - Server close.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jimi\OneDrive\Documents\Courses\Fundamental of SWE\3310 Group project\cse3310_sp24_group_12\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/19739d4a924ac107/Documents/University/Spring 2024/Fundamentals of Software Engineering/Project/cse3310_sp24_group_12/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{590C3224-3FCA-41FC-A065-5B8D8B1CDAA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{590C3224-3FCA-41FC-A065-5B8D8B1CDAA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A49D8B86-8845-4569-8459-330558F51C09}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="26">
   <si>
     <t>Action</t>
   </si>
@@ -90,9 +90,6 @@
     <t>Players are taken to game screen at the end of 5 second countdown</t>
   </si>
   <si>
-    <t>Server is forced to stop</t>
-  </si>
-  <si>
     <t>All timers and intevals should stop, all displays should disapear, Server offline screen should display</t>
   </si>
   <si>
@@ -100,13 +97,19 @@
   </si>
   <si>
     <t>SREQ009/SREQ037</t>
+  </si>
+  <si>
+    <t>Server is forced to stop (using ctrl+c)</t>
+  </si>
+  <si>
+    <t>SREQ045</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -144,6 +147,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -186,23 +195,23 @@
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -487,387 +496,406 @@
   <dimension ref="A1:P18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:P18"/>
+      <selection activeCell="P20" sqref="P20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5" t="s">
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="6" t="s">
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6" t="s">
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="N1" s="6"/>
-      <c r="O1" s="6"/>
-      <c r="P1" s="6"/>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A2" s="5"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6"/>
-      <c r="N2" s="6"/>
-      <c r="O2" s="6"/>
-      <c r="P2" s="6"/>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A3" s="4" t="s">
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4" t="s">
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4" t="s">
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
-      <c r="M3" s="4" t="s">
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="N3" s="4"/>
-      <c r="O3" s="4"/>
-      <c r="P3" s="4"/>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A4" s="4"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="4"/>
-      <c r="L4" s="4"/>
-      <c r="M4" s="4"/>
-      <c r="N4" s="4"/>
-      <c r="O4" s="4"/>
-      <c r="P4" s="4"/>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
+      <c r="N3" s="3"/>
+      <c r="O3" s="3"/>
+      <c r="P3" s="3"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
+      <c r="P4" s="3"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1" t="s">
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="4" t="s">
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="J5" s="4"/>
-      <c r="K5" s="4"/>
-      <c r="L5" s="4"/>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
-      <c r="L6" s="4"/>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A7" s="1" t="s">
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="3" t="s">
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3" t="s">
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
-      <c r="L7" s="3"/>
-      <c r="M7" s="4" t="s">
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="5"/>
+      <c r="M7" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="N7" s="4"/>
-      <c r="O7" s="4"/>
-      <c r="P7" s="4"/>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
-      <c r="L8" s="3"/>
-      <c r="M8" s="4"/>
-      <c r="N8" s="4"/>
-      <c r="O8" s="4"/>
-      <c r="P8" s="4"/>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A9" s="4" t="s">
+      <c r="N7" s="3"/>
+      <c r="O7" s="3"/>
+      <c r="P7" s="3"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="5"/>
+      <c r="M8" s="3"/>
+      <c r="N8" s="3"/>
+      <c r="O8" s="3"/>
+      <c r="P8" s="3"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4" t="s">
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4" t="s">
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="J9" s="4"/>
-      <c r="K9" s="4"/>
-      <c r="L9" s="4"/>
-      <c r="M9" s="4" t="s">
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="N9" s="4"/>
-      <c r="O9" s="4"/>
-      <c r="P9" s="4"/>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
-      <c r="J10" s="4"/>
-      <c r="K10" s="4"/>
-      <c r="L10" s="4"/>
-      <c r="M10" s="4"/>
-      <c r="N10" s="4"/>
-      <c r="O10" s="4"/>
-      <c r="P10" s="4"/>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A11" s="1" t="s">
+      <c r="N9" s="3"/>
+      <c r="O9" s="3"/>
+      <c r="P9" s="3"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="3"/>
+      <c r="N10" s="3"/>
+      <c r="O10" s="3"/>
+      <c r="P10" s="3"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1" t="s">
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="4" t="s">
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="J11" s="4"/>
-      <c r="K11" s="4"/>
-      <c r="L11" s="4"/>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="4"/>
-      <c r="J12" s="4"/>
-      <c r="K12" s="4"/>
-      <c r="L12" s="4"/>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A13" s="1" t="s">
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12" s="4"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="3" t="s">
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3" t="s">
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="J13" s="3"/>
-      <c r="K13" s="3"/>
-      <c r="L13" s="3"/>
-      <c r="M13" s="4" t="s">
+      <c r="J13" s="5"/>
+      <c r="K13" s="5"/>
+      <c r="L13" s="5"/>
+      <c r="M13" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="N13" s="4"/>
-      <c r="O13" s="4"/>
-      <c r="P13" s="4"/>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
-      <c r="J14" s="3"/>
-      <c r="K14" s="3"/>
-      <c r="L14" s="3"/>
-      <c r="M14" s="4"/>
-      <c r="N14" s="4"/>
-      <c r="O14" s="4"/>
-      <c r="P14" s="4"/>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A15" s="1" t="s">
+      <c r="N13" s="3"/>
+      <c r="O13" s="3"/>
+      <c r="P13" s="3"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" s="4"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="5"/>
+      <c r="K14" s="5"/>
+      <c r="L14" s="5"/>
+      <c r="M14" s="3"/>
+      <c r="N14" s="3"/>
+      <c r="O14" s="3"/>
+      <c r="P14" s="3"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="3" t="s">
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3" t="s">
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J15" s="3"/>
-      <c r="K15" s="3"/>
-      <c r="L15" s="3"/>
-      <c r="M15" s="4" t="s">
+      <c r="J15" s="5"/>
+      <c r="K15" s="5"/>
+      <c r="L15" s="5"/>
+      <c r="M15" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="N15" s="3"/>
+      <c r="O15" s="3"/>
+      <c r="P15" s="3"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A16" s="4"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="5"/>
+      <c r="K16" s="5"/>
+      <c r="L16" s="5"/>
+      <c r="M16" s="3"/>
+      <c r="N16" s="3"/>
+      <c r="O16" s="3"/>
+      <c r="P16" s="3"/>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="N15" s="4"/>
-      <c r="O15" s="4"/>
-      <c r="P15" s="4"/>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
-      <c r="J16" s="3"/>
-      <c r="K16" s="3"/>
-      <c r="L16" s="3"/>
-      <c r="M16" s="4"/>
-      <c r="N16" s="4"/>
-      <c r="O16" s="4"/>
-      <c r="P16" s="4"/>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A17" s="1" t="s">
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="2" t="s">
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="J17" s="2"/>
-      <c r="K17" s="2"/>
-      <c r="L17" s="2"/>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
-      <c r="I18" s="2"/>
-      <c r="J18" s="2"/>
-      <c r="K18" s="2"/>
-      <c r="L18" s="2"/>
+      <c r="J17" s="6"/>
+      <c r="K17" s="6"/>
+      <c r="L17" s="6"/>
+      <c r="M17" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="N17" s="3"/>
+      <c r="O17" s="3"/>
+      <c r="P17" s="3"/>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A18" s="4"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="6"/>
+      <c r="J18" s="6"/>
+      <c r="K18" s="6"/>
+      <c r="L18" s="6"/>
+      <c r="M18" s="3"/>
+      <c r="N18" s="3"/>
+      <c r="O18" s="3"/>
+      <c r="P18" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="33">
-    <mergeCell ref="A1:D2"/>
-    <mergeCell ref="E1:H2"/>
-    <mergeCell ref="I1:L2"/>
-    <mergeCell ref="M1:P2"/>
-    <mergeCell ref="A3:D4"/>
-    <mergeCell ref="E3:H4"/>
-    <mergeCell ref="I3:L4"/>
-    <mergeCell ref="M3:P4"/>
+  <mergeCells count="34">
+    <mergeCell ref="M17:P18"/>
+    <mergeCell ref="A17:D18"/>
+    <mergeCell ref="E17:H18"/>
+    <mergeCell ref="I17:L18"/>
+    <mergeCell ref="A13:D14"/>
+    <mergeCell ref="E13:H14"/>
+    <mergeCell ref="I13:L14"/>
+    <mergeCell ref="M13:P14"/>
+    <mergeCell ref="A15:D16"/>
+    <mergeCell ref="E15:H16"/>
+    <mergeCell ref="I15:L16"/>
+    <mergeCell ref="M15:P16"/>
+    <mergeCell ref="M7:P8"/>
+    <mergeCell ref="A9:D10"/>
+    <mergeCell ref="E9:H10"/>
+    <mergeCell ref="I9:L10"/>
+    <mergeCell ref="M9:P10"/>
     <mergeCell ref="A11:D12"/>
     <mergeCell ref="E11:H12"/>
     <mergeCell ref="I11:L12"/>
@@ -877,23 +905,17 @@
     <mergeCell ref="A7:D8"/>
     <mergeCell ref="E7:H8"/>
     <mergeCell ref="I7:L8"/>
-    <mergeCell ref="M7:P8"/>
-    <mergeCell ref="A9:D10"/>
-    <mergeCell ref="E9:H10"/>
-    <mergeCell ref="I9:L10"/>
-    <mergeCell ref="M9:P10"/>
-    <mergeCell ref="M13:P14"/>
-    <mergeCell ref="A15:D16"/>
-    <mergeCell ref="E15:H16"/>
-    <mergeCell ref="I15:L16"/>
-    <mergeCell ref="M15:P16"/>
-    <mergeCell ref="A17:D18"/>
-    <mergeCell ref="E17:H18"/>
-    <mergeCell ref="I17:L18"/>
-    <mergeCell ref="A13:D14"/>
-    <mergeCell ref="E13:H14"/>
-    <mergeCell ref="I13:L14"/>
+    <mergeCell ref="A1:D2"/>
+    <mergeCell ref="E1:H2"/>
+    <mergeCell ref="I1:L2"/>
+    <mergeCell ref="M1:P2"/>
+    <mergeCell ref="A3:D4"/>
+    <mergeCell ref="E3:H4"/>
+    <mergeCell ref="I3:L4"/>
+    <mergeCell ref="M3:P4"/>
   </mergeCells>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>